<commit_message>
test for multiple GHE scenarios
</commit_message>
<xml_diff>
--- a/results/GHP_results.xlsx
+++ b/results/GHP_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Building Name</t>
   </si>
@@ -58,13 +58,16 @@
     <t>Annual Emissions [tonnes CO2]</t>
   </si>
   <si>
-    <t>buildingGHP_district</t>
-  </si>
-  <si>
-    <t>buildingGHP_building_2</t>
-  </si>
-  <si>
-    <t>buildingGHP_building_1</t>
+    <t>building/ghx_GHX_shkwfn</t>
+  </si>
+  <si>
+    <t>building/ghx_GHP_building_mksuwer</t>
+  </si>
+  <si>
+    <t>building/ghx_GHP_building_sdupkgra</t>
+  </si>
+  <si>
+    <t>building/ghx_GHX_ahudfd</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -477,10 +480,10 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>76897.861</v>
+        <v>77335.30809999999</v>
       </c>
       <c r="C2">
-        <v>80956.33</v>
+        <v>81472.3</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -489,7 +492,7 @@
         <v>42.15</v>
       </c>
       <c r="F2">
-        <v>80956.33</v>
+        <v>81472.3</v>
       </c>
       <c r="G2">
         <v>8261.8833</v>
@@ -498,10 +501,10 @@
         <v>66.18000000000001</v>
       </c>
       <c r="I2">
-        <v>1.359</v>
+        <v>1.812</v>
       </c>
       <c r="J2">
-        <v>80956.33</v>
+        <v>81472.3</v>
       </c>
       <c r="K2">
         <v>437.6631368059719</v>
@@ -521,10 +524,10 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <v>18118.1963</v>
+        <v>18062.1037</v>
       </c>
       <c r="C3">
-        <v>8376.6176</v>
+        <v>8320.525</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -533,7 +536,7 @@
         <v>84.29000000000001</v>
       </c>
       <c r="F3">
-        <v>8376.6176</v>
+        <v>8320.525</v>
       </c>
       <c r="G3">
         <v>9741.5787</v>
@@ -542,10 +545,10 @@
         <v>132.37</v>
       </c>
       <c r="I3">
-        <v>1.347</v>
+        <v>2.785</v>
       </c>
       <c r="J3">
-        <v>8376.6176</v>
+        <v>8320.525</v>
       </c>
       <c r="K3">
         <v>437.6631368059719</v>
@@ -565,10 +568,10 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>240076.0547</v>
+        <v>238067.3911</v>
       </c>
       <c r="C4">
-        <v>49971.1648</v>
+        <v>47962.5012</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -577,7 +580,7 @@
         <v>5085.33</v>
       </c>
       <c r="F4">
-        <v>49971.1648</v>
+        <v>47962.5012</v>
       </c>
       <c r="G4">
         <v>190104.8899</v>
@@ -586,10 +589,10 @@
         <v>7779.66</v>
       </c>
       <c r="I4">
-        <v>2.783</v>
+        <v>1.384</v>
       </c>
       <c r="J4">
-        <v>49971.1648</v>
+        <v>47962.5012</v>
       </c>
       <c r="K4">
         <v>26592.59413730094</v>
@@ -602,6 +605,50 @@
       </c>
       <c r="N4">
         <v>7.882400000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>77335.30809999999</v>
+      </c>
+      <c r="C5">
+        <v>81472.3</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>42.15</v>
+      </c>
+      <c r="F5">
+        <v>81472.3</v>
+      </c>
+      <c r="G5">
+        <v>8261.8833</v>
+      </c>
+      <c r="H5">
+        <v>66.18000000000001</v>
+      </c>
+      <c r="I5">
+        <v>1.398</v>
+      </c>
+      <c r="J5">
+        <v>81472.3</v>
+      </c>
+      <c r="K5">
+        <v>437.6631368059719</v>
+      </c>
+      <c r="L5">
+        <v>761.27</v>
+      </c>
+      <c r="M5">
+        <v>1.68</v>
+      </c>
+      <c r="N5">
+        <v>0.0672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>